<commit_message>
Update testcase for allow session + addressing mode + suppress bit for service 22, 2e, 27, 28, 85, 3e;Update database in service 22, 2e : add Allow Session table; Update the position of step TesterPresent at all service (first step is TesterPresent ON, last step is Tester Presend OFF); add Condition check function of testcase for service 3e: vehicle speed, engine status; add column 'Name' in condition table; fix bug from load data and save data process; edit color of testcase file;
</commit_message>
<xml_diff>
--- a/dcomtestcasegeneration/Document/GACA18YBL05V5DCOM Full test except for service 19, 28, 27(5R1V)_FVGTHREEGAC-2639.xlsx
+++ b/dcomtestcasegeneration/Document/GACA18YBL05V5DCOM Full test except for service 19, 28, 27(5R1V)_FVGTHREEGAC-2639.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HuyNA_repo\dcomtestcasegeneration\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D0E31D5-4B8F-4267-9CED-FDBAB424EE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E3317F-4E0B-482B-A382-B8E8C9BF79C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="2355" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCOM" sheetId="12" r:id="rId1"/>
@@ -5679,15 +5679,6 @@
 10) SetEnvVar(string Name EnvTesterPresentOnOff, string Value 0, int WaitTime 1000)</t>
   </si>
   <si>
-    <t>1) Set the   E_pubc_BCS_BCS_2_A_BCS_VehSpd_Pv to   Value 1.5 and   Wait 100 ms
-2) Send 14ffffff Using Physical addressing
-3) Set the   E_pubc_BCS_BCS_2_A_BCS_VehSpd_Pv to   Value 0 and   Wait 100 ms
-4) Set the   E_pubc_BCS_BCS_2_A_BCS_VehSpdVD_Rv to   Value 0 and   Wait 100 ms
-5) Send 14ffffff Using Physical addressing
-6) Set the   E_pubc_BCS_BCS_2_A_BCS_VehSpdVD_Rv to   Value 1 and   Wait 100 ms
-7) Send 14ffffff Using Physical addressing</t>
-  </si>
-  <si>
     <t>1) SetEnvVar(string Name E_pubc_BCS_BCS_2_A_BCS_VehSpd_Pv, string Value 1.5, int WaitTime 100)
 2) RequestResponse(14ffffff, 54, Equal)
 3) SetEnvVar(string Name E_pubc_BCS_BCS_2_A_BCS_VehSpd_Pv, string Value 0, int WaitTime 100)
@@ -15642,6 +15633,15 @@
 94) FunctionalMessage(220e14, 620e14.{2}, Regexp)
 95) DiagSessionCtrl(Default)
 96) SetEnvVar(string Name EnvTesterPresentOnOff, string Value 0, int WaitTime 1000)</t>
+  </si>
+  <si>
+    <t>1) Set the   E_pubc_BCS_BCS_2_A_BCS_VehSpd_Pv to   Value 1.5 and   Wait 100 ms
+2) Send 14ffffff Using Physical addressing
+3) Set the   E_pubc_BCS_BCS_2_A_BCS_VehSpd_Pv to   Value 0  and   Wait 100 ms
+4) Set the   E_pubc_BCS_BCS_2_A_BCS_VehSpdVD_Rv to   Value 0 and   Wait 100 ms
+5) Send 14ffffff Using Physical addressing
+6) Set the   E_pubc_BCS_BCS_2_A_BCS_VehSpdVD_Rv to   Value 1 and   Wait 100 ms
+7) Send 14ffffff Using Physical addressing</t>
   </si>
 </sst>
 </file>
@@ -16138,7 +16138,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -16344,6 +16344,9 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -16364,12 +16367,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -17492,8 +17489,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:M260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="E174" sqref="E174"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17705,13 +17702,13 @@
         <v>83</v>
       </c>
       <c r="C10" s="61" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D10" s="61" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E10" s="61" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="F10" s="61" t="s">
         <v>12</v>
@@ -17720,21 +17717,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="62" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="60">
         <v>845047</v>
       </c>
       <c r="B11" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="90" t="s">
-        <v>743</v>
+      <c r="C11" s="61" t="s">
+        <v>742</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>745</v>
-      </c>
-      <c r="E11" s="90" t="s">
-        <v>747</v>
+        <v>744</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>746</v>
       </c>
       <c r="F11" s="61" t="s">
         <v>12</v>
@@ -17825,13 +17822,13 @@
         <v>65</v>
       </c>
       <c r="C14" s="63" t="s">
+        <v>501</v>
+      </c>
+      <c r="D14" s="63" t="s">
         <v>502</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="E14" s="63" t="s">
         <v>503</v>
-      </c>
-      <c r="E14" s="63" t="s">
-        <v>504</v>
       </c>
       <c r="F14" s="63" t="s">
         <v>12</v>
@@ -18001,7 +17998,7 @@
         <v>12</v>
       </c>
       <c r="G18" s="63" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H18" s="63" t="s">
         <v>51</v>
@@ -18083,7 +18080,7 @@
         <v>12</v>
       </c>
       <c r="G20" s="63" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="H20" s="63" t="s">
         <v>53</v>
@@ -18109,7 +18106,7 @@
         <v>844253</v>
       </c>
       <c r="B21" s="64" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C21" s="63" t="s">
         <v>120</v>
@@ -18153,13 +18150,13 @@
         <v>72</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D22" s="63" t="s">
         <v>114</v>
       </c>
       <c r="E22" s="63" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F22" s="63" t="s">
         <v>12</v>
@@ -18194,13 +18191,13 @@
         <v>116</v>
       </c>
       <c r="C23" s="63" t="s">
+        <v>569</v>
+      </c>
+      <c r="D23" s="63" t="s">
+        <v>504</v>
+      </c>
+      <c r="E23" s="63" t="s">
         <v>570</v>
-      </c>
-      <c r="D23" s="63" t="s">
-        <v>505</v>
-      </c>
-      <c r="E23" s="63" t="s">
-        <v>571</v>
       </c>
       <c r="F23" s="63" t="s">
         <v>12</v>
@@ -18291,16 +18288,16 @@
         <v>844902</v>
       </c>
       <c r="B26" s="78" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C26" s="63" t="s">
+        <v>531</v>
+      </c>
+      <c r="D26" s="63" t="s">
         <v>532</v>
       </c>
-      <c r="D26" s="63" t="s">
+      <c r="E26" s="63" t="s">
         <v>533</v>
-      </c>
-      <c r="E26" s="63" t="s">
-        <v>534</v>
       </c>
       <c r="F26" s="63" t="s">
         <v>12</v>
@@ -18309,7 +18306,7 @@
         <v>8</v>
       </c>
       <c r="H26" s="63" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I26" s="63" t="s">
         <v>14</v>
@@ -18326,16 +18323,16 @@
         <v>844903</v>
       </c>
       <c r="B27" s="78" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D27" s="63" t="s">
         <v>126</v>
       </c>
       <c r="E27" s="63" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F27" s="63" t="s">
         <v>12</v>
@@ -18344,7 +18341,7 @@
         <v>8</v>
       </c>
       <c r="H27" s="63" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="I27" s="63" t="s">
         <v>14</v>
@@ -18361,16 +18358,16 @@
         <v>844908</v>
       </c>
       <c r="B28" s="78" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D28" s="63" t="s">
         <v>127</v>
       </c>
       <c r="E28" s="63" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F28" s="63" t="s">
         <v>12</v>
@@ -18379,7 +18376,7 @@
         <v>8</v>
       </c>
       <c r="H28" s="63" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="I28" s="63" t="s">
         <v>14</v>
@@ -18396,16 +18393,16 @@
         <v>845035</v>
       </c>
       <c r="B29" s="78" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C29" s="63" t="s">
+        <v>539</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>538</v>
+      </c>
+      <c r="E29" s="63" t="s">
         <v>540</v>
-      </c>
-      <c r="D29" s="63" t="s">
-        <v>539</v>
-      </c>
-      <c r="E29" s="63" t="s">
-        <v>541</v>
       </c>
       <c r="F29" s="63" t="s">
         <v>12</v>
@@ -18431,7 +18428,7 @@
         <v>845041</v>
       </c>
       <c r="B30" s="78" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C30" s="63" t="s">
         <v>128</v>
@@ -18440,7 +18437,7 @@
         <v>129</v>
       </c>
       <c r="E30" s="63" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F30" s="63" t="s">
         <v>12</v>
@@ -18466,16 +18463,16 @@
         <v>845040</v>
       </c>
       <c r="B31" s="78" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D31" s="63" t="s">
         <v>129</v>
       </c>
       <c r="E31" s="63" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F31" s="63" t="s">
         <v>12</v>
@@ -18501,16 +18498,16 @@
         <v>845039</v>
       </c>
       <c r="B32" s="78" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C32" s="63" t="s">
+        <v>541</v>
+      </c>
+      <c r="D32" s="63" t="s">
         <v>542</v>
       </c>
-      <c r="D32" s="63" t="s">
+      <c r="E32" s="63" t="s">
         <v>543</v>
-      </c>
-      <c r="E32" s="63" t="s">
-        <v>544</v>
       </c>
       <c r="F32" s="63" t="s">
         <v>12</v>
@@ -18536,16 +18533,16 @@
         <v>845036</v>
       </c>
       <c r="B33" s="78" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C33" s="63" t="s">
+        <v>544</v>
+      </c>
+      <c r="D33" s="63" t="s">
         <v>545</v>
       </c>
-      <c r="D33" s="63" t="s">
+      <c r="E33" s="63" t="s">
         <v>546</v>
-      </c>
-      <c r="E33" s="63" t="s">
-        <v>547</v>
       </c>
       <c r="F33" s="63" t="s">
         <v>12</v>
@@ -18571,7 +18568,7 @@
         <v>844858</v>
       </c>
       <c r="B34" s="78" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C34" s="63" t="s">
         <v>130</v>
@@ -18606,7 +18603,7 @@
         <v>845034</v>
       </c>
       <c r="B35" s="78" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C35" s="63" t="s">
         <v>133</v>
@@ -18641,7 +18638,7 @@
         <v>845042</v>
       </c>
       <c r="B36" s="78" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C36" s="63" t="s">
         <v>137</v>
@@ -18659,7 +18656,7 @@
         <v>8</v>
       </c>
       <c r="H36" s="63" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="I36" s="63" t="s">
         <v>14</v>
@@ -18676,16 +18673,16 @@
         <v>844898</v>
       </c>
       <c r="B37" s="78" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C37" s="63" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D37" s="65" t="s">
         <v>167</v>
       </c>
       <c r="E37" s="63" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F37" s="63" t="s">
         <v>12</v>
@@ -18711,7 +18708,7 @@
         <v>844899</v>
       </c>
       <c r="B38" s="78" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C38" s="63" t="s">
         <v>139</v>
@@ -18746,7 +18743,7 @@
         <v>845038</v>
       </c>
       <c r="B39" s="78" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C39" s="63" t="s">
         <v>145</v>
@@ -18781,7 +18778,7 @@
         <v>844895</v>
       </c>
       <c r="B40" s="78" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C40" s="63" t="s">
         <v>142</v>
@@ -18825,7 +18822,7 @@
         <v>168</v>
       </c>
       <c r="E41" s="63" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F41" s="63" t="s">
         <v>12</v>
@@ -18851,7 +18848,7 @@
         <v>844666</v>
       </c>
       <c r="B42" s="78" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C42" s="63" t="s">
         <v>148</v>
@@ -18886,7 +18883,7 @@
         <v>844846</v>
       </c>
       <c r="B43" s="78" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C43" s="63" t="s">
         <v>151</v>
@@ -18921,7 +18918,7 @@
         <v>844681</v>
       </c>
       <c r="B44" s="78" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C44" s="63" t="s">
         <v>154</v>
@@ -18956,7 +18953,7 @@
         <v>844851</v>
       </c>
       <c r="B45" s="78" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C45" s="63" t="s">
         <v>157</v>
@@ -18991,7 +18988,7 @@
         <v>844901</v>
       </c>
       <c r="B46" s="78" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C46" s="63" t="s">
         <v>160</v>
@@ -19026,7 +19023,7 @@
         <v>844900</v>
       </c>
       <c r="B47" s="78" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C47" s="63" t="s">
         <v>163</v>
@@ -19035,7 +19032,7 @@
         <v>169</v>
       </c>
       <c r="E47" s="63" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F47" s="63" t="s">
         <v>12</v>
@@ -19061,7 +19058,7 @@
         <v>845031</v>
       </c>
       <c r="B48" s="79" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C48" s="63" t="s">
         <v>164</v>
@@ -19096,16 +19093,16 @@
         <v>845030</v>
       </c>
       <c r="B49" s="81" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C49" s="76" t="s">
+        <v>610</v>
+      </c>
+      <c r="D49" s="76" t="s">
+        <v>590</v>
+      </c>
+      <c r="E49" s="82" t="s">
         <v>611</v>
-      </c>
-      <c r="D49" s="76" t="s">
-        <v>591</v>
-      </c>
-      <c r="E49" s="82" t="s">
-        <v>612</v>
       </c>
       <c r="F49" s="76" t="s">
         <v>12</v>
@@ -19131,16 +19128,16 @@
         <v>845029</v>
       </c>
       <c r="B50" s="79" t="s">
+        <v>719</v>
+      </c>
+      <c r="C50" s="63" t="s">
         <v>720</v>
       </c>
-      <c r="C50" s="63" t="s">
+      <c r="D50" s="63" t="s">
         <v>721</v>
       </c>
-      <c r="D50" s="63" t="s">
+      <c r="E50" s="63" t="s">
         <v>722</v>
-      </c>
-      <c r="E50" s="63" t="s">
-        <v>723</v>
       </c>
       <c r="F50" s="63" t="s">
         <v>12</v>
@@ -19166,7 +19163,7 @@
         <v>845028</v>
       </c>
       <c r="B51" s="79" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C51" s="63" t="s">
         <v>164</v>
@@ -19201,16 +19198,16 @@
         <v>845027</v>
       </c>
       <c r="B52" s="79" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C52" s="63" t="s">
+        <v>612</v>
+      </c>
+      <c r="D52" s="63" t="s">
+        <v>606</v>
+      </c>
+      <c r="E52" s="63" t="s">
         <v>613</v>
-      </c>
-      <c r="D52" s="63" t="s">
-        <v>607</v>
-      </c>
-      <c r="E52" s="63" t="s">
-        <v>614</v>
       </c>
       <c r="F52" s="63" t="s">
         <v>12</v>
@@ -19236,7 +19233,7 @@
         <v>845026</v>
       </c>
       <c r="B53" s="79" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C53" s="63" t="s">
         <v>164</v>
@@ -19271,7 +19268,7 @@
         <v>845025</v>
       </c>
       <c r="B54" s="79" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C54" s="63" t="s">
         <v>164</v>
@@ -19306,16 +19303,16 @@
         <v>844917</v>
       </c>
       <c r="B55" s="79" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C55" s="63" t="s">
+        <v>591</v>
+      </c>
+      <c r="D55" s="63" t="s">
         <v>592</v>
       </c>
-      <c r="D55" s="63" t="s">
+      <c r="E55" s="63" t="s">
         <v>593</v>
-      </c>
-      <c r="E55" s="63" t="s">
-        <v>594</v>
       </c>
       <c r="F55" s="63" t="s">
         <v>12</v>
@@ -19341,16 +19338,16 @@
         <v>844914</v>
       </c>
       <c r="B56" s="79" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C56" s="63" t="s">
         <v>175</v>
       </c>
       <c r="D56" s="63" t="s">
+        <v>549</v>
+      </c>
+      <c r="E56" s="63" t="s">
         <v>550</v>
-      </c>
-      <c r="E56" s="63" t="s">
-        <v>551</v>
       </c>
       <c r="F56" s="63" t="s">
         <v>12</v>
@@ -19376,16 +19373,16 @@
         <v>844913</v>
       </c>
       <c r="B57" s="79" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C57" s="63" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D57" s="63" t="s">
+        <v>629</v>
+      </c>
+      <c r="E57" s="63" t="s">
         <v>630</v>
-      </c>
-      <c r="E57" s="63" t="s">
-        <v>631</v>
       </c>
       <c r="F57" s="63" t="s">
         <v>12</v>
@@ -19411,16 +19408,16 @@
         <v>844910</v>
       </c>
       <c r="B58" s="79" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C58" s="63" t="s">
+        <v>615</v>
+      </c>
+      <c r="D58" s="63" t="s">
+        <v>614</v>
+      </c>
+      <c r="E58" s="63" t="s">
         <v>616</v>
-      </c>
-      <c r="D58" s="63" t="s">
-        <v>615</v>
-      </c>
-      <c r="E58" s="63" t="s">
-        <v>617</v>
       </c>
       <c r="F58" s="63" t="s">
         <v>12</v>
@@ -19446,16 +19443,16 @@
         <v>845033</v>
       </c>
       <c r="B59" s="78" t="s">
+        <v>731</v>
+      </c>
+      <c r="C59" s="63" t="s">
         <v>732</v>
       </c>
-      <c r="C59" s="63" t="s">
+      <c r="D59" s="63" t="s">
         <v>733</v>
       </c>
-      <c r="D59" s="63" t="s">
+      <c r="E59" s="63" t="s">
         <v>734</v>
-      </c>
-      <c r="E59" s="63" t="s">
-        <v>735</v>
       </c>
       <c r="F59" s="63" t="s">
         <v>12</v>
@@ -19481,16 +19478,16 @@
         <v>845032</v>
       </c>
       <c r="B60" s="78" t="s">
+        <v>735</v>
+      </c>
+      <c r="C60" s="63" t="s">
         <v>736</v>
       </c>
-      <c r="C60" s="63" t="s">
+      <c r="D60" s="63" t="s">
         <v>737</v>
       </c>
-      <c r="D60" s="63" t="s">
+      <c r="E60" s="63" t="s">
         <v>738</v>
-      </c>
-      <c r="E60" s="63" t="s">
-        <v>739</v>
       </c>
       <c r="F60" s="63" t="s">
         <v>12</v>
@@ -19516,16 +19513,16 @@
         <v>844905</v>
       </c>
       <c r="B61" s="78" t="s">
+        <v>739</v>
+      </c>
+      <c r="C61" s="63" t="s">
+        <v>552</v>
+      </c>
+      <c r="D61" s="63" t="s">
         <v>740</v>
       </c>
-      <c r="C61" s="63" t="s">
-        <v>553</v>
-      </c>
-      <c r="D61" s="63" t="s">
+      <c r="E61" s="63" t="s">
         <v>741</v>
-      </c>
-      <c r="E61" s="63" t="s">
-        <v>742</v>
       </c>
       <c r="F61" s="63" t="s">
         <v>12</v>
@@ -19926,13 +19923,13 @@
         <v>212</v>
       </c>
       <c r="C73" s="63" t="s">
+        <v>600</v>
+      </c>
+      <c r="D73" s="63" t="s">
         <v>601</v>
       </c>
-      <c r="D73" s="63" t="s">
+      <c r="E73" s="63" t="s">
         <v>602</v>
-      </c>
-      <c r="E73" s="63" t="s">
-        <v>603</v>
       </c>
       <c r="F73" s="63" t="s">
         <v>12</v>
@@ -19961,13 +19958,13 @@
         <v>211</v>
       </c>
       <c r="C74" s="63" t="s">
+        <v>594</v>
+      </c>
+      <c r="D74" s="63" t="s">
         <v>595</v>
       </c>
-      <c r="D74" s="63" t="s">
+      <c r="E74" s="63" t="s">
         <v>596</v>
-      </c>
-      <c r="E74" s="63" t="s">
-        <v>597</v>
       </c>
       <c r="F74" s="63" t="s">
         <v>12</v>
@@ -19996,13 +19993,13 @@
         <v>213</v>
       </c>
       <c r="C75" s="63" t="s">
+        <v>597</v>
+      </c>
+      <c r="D75" s="63" t="s">
         <v>598</v>
       </c>
-      <c r="D75" s="63" t="s">
+      <c r="E75" s="63" t="s">
         <v>599</v>
-      </c>
-      <c r="E75" s="63" t="s">
-        <v>600</v>
       </c>
       <c r="F75" s="63" t="s">
         <v>12</v>
@@ -20031,13 +20028,13 @@
         <v>186</v>
       </c>
       <c r="C76" s="63" t="s">
+        <v>603</v>
+      </c>
+      <c r="D76" s="65" t="s">
         <v>604</v>
       </c>
-      <c r="D76" s="65" t="s">
+      <c r="E76" s="63" t="s">
         <v>605</v>
-      </c>
-      <c r="E76" s="63" t="s">
-        <v>606</v>
       </c>
       <c r="F76" s="63" t="s">
         <v>12</v>
@@ -20328,14 +20325,14 @@
       </c>
       <c r="L84" s="65"/>
     </row>
-    <row r="85" spans="1:13" s="62" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" s="62" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A85" s="67">
         <v>845120</v>
       </c>
       <c r="B85" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="C85" s="63" t="s">
+      <c r="C85" s="83" t="s">
         <v>245</v>
       </c>
       <c r="D85" s="63" t="s">
@@ -20510,13 +20507,13 @@
         <v>251</v>
       </c>
       <c r="C90" s="63" t="s">
-        <v>361</v>
+        <v>748</v>
       </c>
       <c r="D90" s="65" t="s">
         <v>266</v>
       </c>
       <c r="E90" s="63" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F90" s="63" t="s">
         <v>12</v>
@@ -20548,13 +20545,13 @@
         <v>252</v>
       </c>
       <c r="C91" s="67" t="s">
+        <v>573</v>
+      </c>
+      <c r="D91" s="65" t="s">
         <v>574</v>
       </c>
-      <c r="D91" s="65" t="s">
+      <c r="E91" s="63" t="s">
         <v>575</v>
-      </c>
-      <c r="E91" s="63" t="s">
-        <v>576</v>
       </c>
       <c r="F91" s="63" t="s">
         <v>12</v>
@@ -20681,13 +20678,13 @@
         <v>275</v>
       </c>
       <c r="C95" s="68" t="s">
+        <v>553</v>
+      </c>
+      <c r="D95" s="65" t="s">
         <v>554</v>
       </c>
-      <c r="D95" s="65" t="s">
+      <c r="E95" s="63" t="s">
         <v>555</v>
-      </c>
-      <c r="E95" s="63" t="s">
-        <v>556</v>
       </c>
       <c r="F95" s="63" t="s">
         <v>12</v>
@@ -20716,13 +20713,13 @@
         <v>276</v>
       </c>
       <c r="C96" s="68" t="s">
+        <v>556</v>
+      </c>
+      <c r="D96" s="63" t="s">
         <v>557</v>
       </c>
-      <c r="D96" s="63" t="s">
+      <c r="E96" s="63" t="s">
         <v>558</v>
-      </c>
-      <c r="E96" s="63" t="s">
-        <v>559</v>
       </c>
       <c r="F96" s="63" t="s">
         <v>12</v>
@@ -20751,13 +20748,13 @@
         <v>62</v>
       </c>
       <c r="C97" s="68" t="s">
+        <v>559</v>
+      </c>
+      <c r="D97" s="63" t="s">
         <v>560</v>
       </c>
-      <c r="D97" s="63" t="s">
+      <c r="E97" s="63" t="s">
         <v>561</v>
-      </c>
-      <c r="E97" s="63" t="s">
-        <v>562</v>
       </c>
       <c r="F97" s="63" t="s">
         <v>12</v>
@@ -20961,13 +20958,13 @@
         <v>270</v>
       </c>
       <c r="C103" s="68" t="s">
+        <v>562</v>
+      </c>
+      <c r="D103" s="63" t="s">
         <v>563</v>
       </c>
-      <c r="D103" s="63" t="s">
+      <c r="E103" s="63" t="s">
         <v>564</v>
-      </c>
-      <c r="E103" s="63" t="s">
-        <v>565</v>
       </c>
       <c r="F103" s="63" t="s">
         <v>12</v>
@@ -21017,13 +21014,13 @@
         <v>306</v>
       </c>
       <c r="C105" s="63" t="s">
+        <v>526</v>
+      </c>
+      <c r="D105" s="63" t="s">
         <v>527</v>
       </c>
-      <c r="D105" s="63" t="s">
+      <c r="E105" s="63" t="s">
         <v>528</v>
-      </c>
-      <c r="E105" s="63" t="s">
-        <v>529</v>
       </c>
       <c r="F105" s="63" t="s">
         <v>12</v>
@@ -21052,13 +21049,13 @@
         <v>307</v>
       </c>
       <c r="C106" s="67" t="s">
+        <v>565</v>
+      </c>
+      <c r="D106" s="67" t="s">
         <v>566</v>
       </c>
-      <c r="D106" s="67" t="s">
+      <c r="E106" s="63" t="s">
         <v>567</v>
-      </c>
-      <c r="E106" s="63" t="s">
-        <v>568</v>
       </c>
       <c r="F106" s="63" t="s">
         <v>12</v>
@@ -21087,13 +21084,13 @@
         <v>308</v>
       </c>
       <c r="C107" s="67" t="s">
+        <v>617</v>
+      </c>
+      <c r="D107" s="67" t="s">
         <v>618</v>
       </c>
-      <c r="D107" s="67" t="s">
+      <c r="E107" s="63" t="s">
         <v>619</v>
-      </c>
-      <c r="E107" s="63" t="s">
-        <v>620</v>
       </c>
       <c r="F107" s="63" t="s">
         <v>12</v>
@@ -21227,13 +21224,13 @@
         <v>296</v>
       </c>
       <c r="C111" s="67" t="s">
+        <v>620</v>
+      </c>
+      <c r="D111" s="67" t="s">
         <v>621</v>
       </c>
-      <c r="D111" s="67" t="s">
+      <c r="E111" s="63" t="s">
         <v>622</v>
-      </c>
-      <c r="E111" s="63" t="s">
-        <v>623</v>
       </c>
       <c r="F111" s="63" t="s">
         <v>12</v>
@@ -21262,13 +21259,13 @@
         <v>297</v>
       </c>
       <c r="C112" s="67" t="s">
+        <v>623</v>
+      </c>
+      <c r="D112" s="67" t="s">
+        <v>621</v>
+      </c>
+      <c r="E112" s="63" t="s">
         <v>624</v>
-      </c>
-      <c r="D112" s="67" t="s">
-        <v>622</v>
-      </c>
-      <c r="E112" s="63" t="s">
-        <v>625</v>
       </c>
       <c r="F112" s="63" t="s">
         <v>12</v>
@@ -21297,13 +21294,13 @@
         <v>315</v>
       </c>
       <c r="C113" s="68" t="s">
+        <v>576</v>
+      </c>
+      <c r="D113" s="63" t="s">
         <v>577</v>
       </c>
-      <c r="D113" s="63" t="s">
+      <c r="E113" s="63" t="s">
         <v>578</v>
-      </c>
-      <c r="E113" s="63" t="s">
-        <v>579</v>
       </c>
       <c r="F113" s="63" t="s">
         <v>12</v>
@@ -21332,13 +21329,13 @@
         <v>316</v>
       </c>
       <c r="C114" s="65" t="s">
+        <v>579</v>
+      </c>
+      <c r="D114" s="65" t="s">
+        <v>577</v>
+      </c>
+      <c r="E114" s="63" t="s">
         <v>580</v>
-      </c>
-      <c r="D114" s="65" t="s">
-        <v>578</v>
-      </c>
-      <c r="E114" s="63" t="s">
-        <v>581</v>
       </c>
       <c r="F114" s="63" t="s">
         <v>12</v>
@@ -21367,13 +21364,13 @@
         <v>302</v>
       </c>
       <c r="C115" s="67" t="s">
+        <v>508</v>
+      </c>
+      <c r="D115" s="67" t="s">
         <v>509</v>
       </c>
-      <c r="D115" s="67" t="s">
+      <c r="E115" s="63" t="s">
         <v>510</v>
-      </c>
-      <c r="E115" s="63" t="s">
-        <v>511</v>
       </c>
       <c r="F115" s="63" t="s">
         <v>12</v>
@@ -21402,13 +21399,13 @@
         <v>303</v>
       </c>
       <c r="C116" s="67" t="s">
+        <v>511</v>
+      </c>
+      <c r="D116" s="67" t="s">
         <v>512</v>
       </c>
-      <c r="D116" s="67" t="s">
+      <c r="E116" s="63" t="s">
         <v>513</v>
-      </c>
-      <c r="E116" s="63" t="s">
-        <v>514</v>
       </c>
       <c r="F116" s="63" t="s">
         <v>12</v>
@@ -21437,13 +21434,13 @@
         <v>301</v>
       </c>
       <c r="C117" s="67" t="s">
+        <v>514</v>
+      </c>
+      <c r="D117" s="67" t="s">
         <v>515</v>
       </c>
-      <c r="D117" s="67" t="s">
+      <c r="E117" s="63" t="s">
         <v>516</v>
-      </c>
-      <c r="E117" s="63" t="s">
-        <v>517</v>
       </c>
       <c r="F117" s="63" t="s">
         <v>12</v>
@@ -21472,13 +21469,13 @@
         <v>300</v>
       </c>
       <c r="C118" s="63" t="s">
+        <v>517</v>
+      </c>
+      <c r="D118" s="67" t="s">
         <v>518</v>
       </c>
-      <c r="D118" s="67" t="s">
+      <c r="E118" s="63" t="s">
         <v>519</v>
-      </c>
-      <c r="E118" s="63" t="s">
-        <v>520</v>
       </c>
       <c r="F118" s="63" t="s">
         <v>12</v>
@@ -21507,13 +21504,13 @@
         <v>304</v>
       </c>
       <c r="C119" s="67" t="s">
+        <v>520</v>
+      </c>
+      <c r="D119" s="67" t="s">
         <v>521</v>
       </c>
-      <c r="D119" s="67" t="s">
+      <c r="E119" s="63" t="s">
         <v>522</v>
-      </c>
-      <c r="E119" s="63" t="s">
-        <v>523</v>
       </c>
       <c r="F119" s="63" t="s">
         <v>12</v>
@@ -21542,13 +21539,13 @@
         <v>299</v>
       </c>
       <c r="C120" s="63" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D120" s="63" t="s">
+        <v>625</v>
+      </c>
+      <c r="E120" s="63" t="s">
         <v>626</v>
-      </c>
-      <c r="E120" s="63" t="s">
-        <v>627</v>
       </c>
       <c r="F120" s="63" t="s">
         <v>12</v>
@@ -21577,13 +21574,13 @@
         <v>298</v>
       </c>
       <c r="C121" s="63" t="s">
+        <v>523</v>
+      </c>
+      <c r="D121" s="63" t="s">
         <v>524</v>
       </c>
-      <c r="D121" s="63" t="s">
+      <c r="E121" s="63" t="s">
         <v>525</v>
-      </c>
-      <c r="E121" s="63" t="s">
-        <v>526</v>
       </c>
       <c r="F121" s="63" t="s">
         <v>12</v>
@@ -21632,13 +21629,13 @@
         <v>328</v>
       </c>
       <c r="C123" s="63" t="s">
+        <v>492</v>
+      </c>
+      <c r="D123" s="63" t="s">
         <v>493</v>
       </c>
-      <c r="D123" s="63" t="s">
+      <c r="E123" s="63" t="s">
         <v>494</v>
-      </c>
-      <c r="E123" s="63" t="s">
-        <v>495</v>
       </c>
       <c r="F123" s="63" t="s">
         <v>12</v>
@@ -21667,13 +21664,13 @@
         <v>329</v>
       </c>
       <c r="C124" s="67" t="s">
+        <v>495</v>
+      </c>
+      <c r="D124" s="67" t="s">
         <v>496</v>
       </c>
-      <c r="D124" s="67" t="s">
+      <c r="E124" s="63" t="s">
         <v>497</v>
-      </c>
-      <c r="E124" s="63" t="s">
-        <v>498</v>
       </c>
       <c r="F124" s="63" t="s">
         <v>12</v>
@@ -21702,13 +21699,13 @@
         <v>330</v>
       </c>
       <c r="C125" s="67" t="s">
+        <v>498</v>
+      </c>
+      <c r="D125" s="67" t="s">
         <v>499</v>
       </c>
-      <c r="D125" s="67" t="s">
+      <c r="E125" s="63" t="s">
         <v>500</v>
-      </c>
-      <c r="E125" s="63" t="s">
-        <v>501</v>
       </c>
       <c r="F125" s="63" t="s">
         <v>12</v>
@@ -21772,13 +21769,13 @@
         <v>334</v>
       </c>
       <c r="C127" s="63" t="s">
+        <v>367</v>
+      </c>
+      <c r="D127" s="63" t="s">
         <v>368</v>
       </c>
-      <c r="D127" s="63" t="s">
+      <c r="E127" s="63" t="s">
         <v>369</v>
-      </c>
-      <c r="E127" s="63" t="s">
-        <v>370</v>
       </c>
       <c r="F127" s="63" t="s">
         <v>12</v>
@@ -21982,13 +21979,13 @@
         <v>336</v>
       </c>
       <c r="C133" s="67" t="s">
+        <v>364</v>
+      </c>
+      <c r="D133" s="67" t="s">
         <v>365</v>
       </c>
-      <c r="D133" s="67" t="s">
+      <c r="E133" s="63" t="s">
         <v>366</v>
-      </c>
-      <c r="E133" s="63" t="s">
-        <v>367</v>
       </c>
       <c r="F133" s="63" t="s">
         <v>12</v>
@@ -22052,13 +22049,13 @@
         <v>333</v>
       </c>
       <c r="C135" s="67" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D135" s="67" t="s">
         <v>358</v>
       </c>
       <c r="E135" s="63" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F135" s="63" t="s">
         <v>12</v>
@@ -22087,13 +22084,13 @@
         <v>331</v>
       </c>
       <c r="C136" s="68" t="s">
+        <v>581</v>
+      </c>
+      <c r="D136" s="63" t="s">
         <v>582</v>
       </c>
-      <c r="D136" s="63" t="s">
+      <c r="E136" s="63" t="s">
         <v>583</v>
-      </c>
-      <c r="E136" s="63" t="s">
-        <v>584</v>
       </c>
       <c r="F136" s="63" t="s">
         <v>12</v>
@@ -22122,13 +22119,13 @@
         <v>332</v>
       </c>
       <c r="C137" s="65" t="s">
+        <v>584</v>
+      </c>
+      <c r="D137" s="65" t="s">
+        <v>582</v>
+      </c>
+      <c r="E137" s="63" t="s">
         <v>585</v>
-      </c>
-      <c r="D137" s="65" t="s">
-        <v>583</v>
-      </c>
-      <c r="E137" s="63" t="s">
-        <v>586</v>
       </c>
       <c r="F137" s="63" t="s">
         <v>12</v>
@@ -22192,13 +22189,13 @@
         <v>320</v>
       </c>
       <c r="C139" s="67" t="s">
+        <v>386</v>
+      </c>
+      <c r="D139" s="67" t="s">
         <v>387</v>
       </c>
-      <c r="D139" s="67" t="s">
+      <c r="E139" s="63" t="s">
         <v>388</v>
-      </c>
-      <c r="E139" s="63" t="s">
-        <v>389</v>
       </c>
       <c r="F139" s="63" t="s">
         <v>12</v>
@@ -22247,16 +22244,16 @@
         <v>845106</v>
       </c>
       <c r="B141" s="67" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C141" s="67" t="s">
+        <v>410</v>
+      </c>
+      <c r="D141" s="67" t="s">
         <v>411</v>
       </c>
-      <c r="D141" s="67" t="s">
+      <c r="E141" s="63" t="s">
         <v>412</v>
-      </c>
-      <c r="E141" s="63" t="s">
-        <v>413</v>
       </c>
       <c r="F141" s="63" t="s">
         <v>12</v>
@@ -22282,16 +22279,16 @@
         <v>845105</v>
       </c>
       <c r="B142" s="67" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C142" s="67" t="s">
+        <v>413</v>
+      </c>
+      <c r="D142" s="67" t="s">
         <v>414</v>
       </c>
-      <c r="D142" s="67" t="s">
+      <c r="E142" s="63" t="s">
         <v>415</v>
-      </c>
-      <c r="E142" s="63" t="s">
-        <v>416</v>
       </c>
       <c r="F142" s="63" t="s">
         <v>12</v>
@@ -22317,16 +22314,16 @@
         <v>845104</v>
       </c>
       <c r="B143" s="67" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C143" s="67" t="s">
+        <v>416</v>
+      </c>
+      <c r="D143" s="67" t="s">
         <v>417</v>
       </c>
-      <c r="D143" s="67" t="s">
+      <c r="E143" s="63" t="s">
         <v>418</v>
-      </c>
-      <c r="E143" s="63" t="s">
-        <v>419</v>
       </c>
       <c r="F143" s="63" t="s">
         <v>12</v>
@@ -22352,16 +22349,16 @@
         <v>845103</v>
       </c>
       <c r="B144" s="67" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C144" s="67" t="s">
+        <v>420</v>
+      </c>
+      <c r="D144" s="67" t="s">
+        <v>419</v>
+      </c>
+      <c r="E144" s="63" t="s">
         <v>421</v>
-      </c>
-      <c r="D144" s="67" t="s">
-        <v>420</v>
-      </c>
-      <c r="E144" s="63" t="s">
-        <v>422</v>
       </c>
       <c r="F144" s="63" t="s">
         <v>12</v>
@@ -22387,16 +22384,16 @@
         <v>845102</v>
       </c>
       <c r="B145" s="67" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C145" s="67" t="s">
+        <v>586</v>
+      </c>
+      <c r="D145" s="67" t="s">
+        <v>422</v>
+      </c>
+      <c r="E145" s="63" t="s">
         <v>587</v>
-      </c>
-      <c r="D145" s="67" t="s">
-        <v>423</v>
-      </c>
-      <c r="E145" s="63" t="s">
-        <v>588</v>
       </c>
       <c r="F145" s="63" t="s">
         <v>12</v>
@@ -22422,16 +22419,16 @@
         <v>845101</v>
       </c>
       <c r="B146" s="67" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C146" s="67" t="s">
+        <v>423</v>
+      </c>
+      <c r="D146" s="67" t="s">
         <v>424</v>
       </c>
-      <c r="D146" s="67" t="s">
+      <c r="E146" s="63" t="s">
         <v>425</v>
-      </c>
-      <c r="E146" s="63" t="s">
-        <v>426</v>
       </c>
       <c r="F146" s="63" t="s">
         <v>12</v>
@@ -22457,16 +22454,16 @@
         <v>845100</v>
       </c>
       <c r="B147" s="67" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C147" s="67" t="s">
+        <v>426</v>
+      </c>
+      <c r="D147" s="67" t="s">
         <v>427</v>
       </c>
-      <c r="D147" s="67" t="s">
+      <c r="E147" s="63" t="s">
         <v>428</v>
-      </c>
-      <c r="E147" s="63" t="s">
-        <v>429</v>
       </c>
       <c r="F147" s="63" t="s">
         <v>12</v>
@@ -22492,16 +22489,16 @@
         <v>845099</v>
       </c>
       <c r="B148" s="67" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C148" s="67" t="s">
+        <v>389</v>
+      </c>
+      <c r="D148" s="67" t="s">
         <v>390</v>
       </c>
-      <c r="D148" s="67" t="s">
+      <c r="E148" s="63" t="s">
         <v>391</v>
-      </c>
-      <c r="E148" s="63" t="s">
-        <v>392</v>
       </c>
       <c r="F148" s="63" t="s">
         <v>12</v>
@@ -22527,16 +22524,16 @@
         <v>845098</v>
       </c>
       <c r="B149" s="67" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C149" s="63" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D149" s="63" t="s">
+        <v>649</v>
+      </c>
+      <c r="E149" s="63" t="s">
         <v>650</v>
-      </c>
-      <c r="E149" s="63" t="s">
-        <v>651</v>
       </c>
       <c r="F149" s="63" t="s">
         <v>12</v>
@@ -22562,16 +22559,16 @@
         <v>845097</v>
       </c>
       <c r="B150" s="67" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C150" s="63" t="s">
+        <v>394</v>
+      </c>
+      <c r="D150" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="E150" s="63" t="s">
         <v>395</v>
-      </c>
-      <c r="D150" s="63" t="s">
-        <v>394</v>
-      </c>
-      <c r="E150" s="63" t="s">
-        <v>396</v>
       </c>
       <c r="F150" s="63" t="s">
         <v>12</v>
@@ -22597,16 +22594,16 @@
         <v>845096</v>
       </c>
       <c r="B151" s="67" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C151" s="63" t="s">
+        <v>396</v>
+      </c>
+      <c r="D151" s="63" t="s">
         <v>397</v>
       </c>
-      <c r="D151" s="63" t="s">
+      <c r="E151" s="63" t="s">
         <v>398</v>
-      </c>
-      <c r="E151" s="63" t="s">
-        <v>399</v>
       </c>
       <c r="F151" s="63" t="s">
         <v>12</v>
@@ -22632,16 +22629,16 @@
         <v>845095</v>
       </c>
       <c r="B152" s="67" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C152" s="63" t="s">
+        <v>627</v>
+      </c>
+      <c r="D152" s="67" t="s">
+        <v>399</v>
+      </c>
+      <c r="E152" s="63" t="s">
         <v>628</v>
-      </c>
-      <c r="D152" s="67" t="s">
-        <v>400</v>
-      </c>
-      <c r="E152" s="63" t="s">
-        <v>629</v>
       </c>
       <c r="F152" s="63" t="s">
         <v>12</v>
@@ -22667,16 +22664,16 @@
         <v>845094</v>
       </c>
       <c r="B153" s="67" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C153" s="67" t="s">
+        <v>400</v>
+      </c>
+      <c r="D153" s="67" t="s">
         <v>401</v>
       </c>
-      <c r="D153" s="67" t="s">
+      <c r="E153" s="63" t="s">
         <v>402</v>
-      </c>
-      <c r="E153" s="63" t="s">
-        <v>403</v>
       </c>
       <c r="F153" s="63" t="s">
         <v>12</v>
@@ -22702,16 +22699,16 @@
         <v>845090</v>
       </c>
       <c r="B154" s="67" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C154" s="67" t="s">
+        <v>403</v>
+      </c>
+      <c r="D154" s="67" t="s">
         <v>404</v>
       </c>
-      <c r="D154" s="67" t="s">
+      <c r="E154" s="63" t="s">
         <v>405</v>
-      </c>
-      <c r="E154" s="63" t="s">
-        <v>406</v>
       </c>
       <c r="F154" s="63" t="s">
         <v>12</v>
@@ -22737,16 +22734,16 @@
         <v>845089</v>
       </c>
       <c r="B155" s="67" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C155" s="67" t="s">
+        <v>588</v>
+      </c>
+      <c r="D155" s="67" t="s">
+        <v>406</v>
+      </c>
+      <c r="E155" s="63" t="s">
         <v>589</v>
-      </c>
-      <c r="D155" s="67" t="s">
-        <v>407</v>
-      </c>
-      <c r="E155" s="63" t="s">
-        <v>590</v>
       </c>
       <c r="F155" s="63" t="s">
         <v>12</v>
@@ -22772,16 +22769,16 @@
         <v>845088</v>
       </c>
       <c r="B156" s="67" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C156" s="63" t="s">
+        <v>407</v>
+      </c>
+      <c r="D156" s="63" t="s">
         <v>408</v>
       </c>
-      <c r="D156" s="63" t="s">
+      <c r="E156" s="63" t="s">
         <v>409</v>
-      </c>
-      <c r="E156" s="63" t="s">
-        <v>410</v>
       </c>
       <c r="F156" s="63" t="s">
         <v>12</v>
@@ -22822,21 +22819,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:11" s="65" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="67">
         <v>845137</v>
       </c>
       <c r="B158" s="67" t="s">
-        <v>430</v>
-      </c>
-      <c r="C158" s="91" t="s">
+        <v>429</v>
+      </c>
+      <c r="C158" s="63" t="s">
+        <v>446</v>
+      </c>
+      <c r="D158" s="65" t="s">
         <v>447</v>
       </c>
-      <c r="D158" s="65" t="s">
+      <c r="E158" s="63" t="s">
         <v>448</v>
-      </c>
-      <c r="E158" s="63" t="s">
-        <v>449</v>
       </c>
       <c r="F158" s="63" t="s">
         <v>12</v>
@@ -22857,21 +22854,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:11" s="65" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="67">
         <v>845138</v>
       </c>
       <c r="B159" s="67" t="s">
-        <v>431</v>
-      </c>
-      <c r="C159" s="91" t="s">
+        <v>430</v>
+      </c>
+      <c r="C159" s="63" t="s">
+        <v>449</v>
+      </c>
+      <c r="D159" s="63" t="s">
         <v>450</v>
       </c>
-      <c r="D159" s="63" t="s">
+      <c r="E159" s="63" t="s">
         <v>451</v>
-      </c>
-      <c r="E159" s="63" t="s">
-        <v>452</v>
       </c>
       <c r="F159" s="63" t="s">
         <v>12</v>
@@ -22897,16 +22894,16 @@
         <v>845134</v>
       </c>
       <c r="B160" s="67" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C160" s="63" t="s">
+        <v>455</v>
+      </c>
+      <c r="D160" s="63" t="s">
         <v>456</v>
       </c>
-      <c r="D160" s="63" t="s">
+      <c r="E160" s="63" t="s">
         <v>457</v>
-      </c>
-      <c r="E160" s="63" t="s">
-        <v>458</v>
       </c>
       <c r="F160" s="63" t="s">
         <v>12</v>
@@ -22932,16 +22929,16 @@
         <v>845133</v>
       </c>
       <c r="B161" s="67" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C161" s="63" t="s">
+        <v>458</v>
+      </c>
+      <c r="D161" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="E161" s="63" t="s">
         <v>459</v>
-      </c>
-      <c r="D161" s="63" t="s">
-        <v>457</v>
-      </c>
-      <c r="E161" s="63" t="s">
-        <v>460</v>
       </c>
       <c r="F161" s="63" t="s">
         <v>12</v>
@@ -22967,16 +22964,16 @@
         <v>874843</v>
       </c>
       <c r="B162" s="67" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C162" s="68" t="s">
+        <v>460</v>
+      </c>
+      <c r="D162" s="63" t="s">
         <v>461</v>
       </c>
-      <c r="D162" s="63" t="s">
+      <c r="E162" s="63" t="s">
         <v>462</v>
-      </c>
-      <c r="E162" s="63" t="s">
-        <v>463</v>
       </c>
       <c r="F162" s="63" t="s">
         <v>12</v>
@@ -23002,16 +22999,16 @@
         <v>874844</v>
       </c>
       <c r="B163" s="67" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C163" s="65" t="s">
+        <v>463</v>
+      </c>
+      <c r="D163" s="65" t="s">
+        <v>461</v>
+      </c>
+      <c r="E163" s="63" t="s">
         <v>464</v>
-      </c>
-      <c r="D163" s="65" t="s">
-        <v>462</v>
-      </c>
-      <c r="E163" s="63" t="s">
-        <v>465</v>
       </c>
       <c r="F163" s="63" t="s">
         <v>12</v>
@@ -23037,16 +23034,16 @@
         <v>845135</v>
       </c>
       <c r="B164" s="67" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C164" s="63" t="s">
+        <v>452</v>
+      </c>
+      <c r="D164" s="63" t="s">
         <v>453</v>
       </c>
-      <c r="D164" s="63" t="s">
+      <c r="E164" s="63" t="s">
         <v>454</v>
-      </c>
-      <c r="E164" s="63" t="s">
-        <v>455</v>
       </c>
       <c r="F164" s="63" t="s">
         <v>12</v>
@@ -23072,16 +23069,16 @@
         <v>845136</v>
       </c>
       <c r="B165" s="67" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C165" s="63" t="s">
+        <v>489</v>
+      </c>
+      <c r="D165" s="65" t="s">
+        <v>491</v>
+      </c>
+      <c r="E165" s="63" t="s">
         <v>490</v>
-      </c>
-      <c r="D165" s="65" t="s">
-        <v>492</v>
-      </c>
-      <c r="E165" s="63" t="s">
-        <v>491</v>
       </c>
       <c r="F165" s="63" t="s">
         <v>12</v>
@@ -23107,16 +23104,16 @@
         <v>845132</v>
       </c>
       <c r="B166" s="67" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C166" s="63" t="s">
+        <v>655</v>
+      </c>
+      <c r="D166" s="65" t="s">
+        <v>657</v>
+      </c>
+      <c r="E166" s="63" t="s">
         <v>656</v>
-      </c>
-      <c r="D166" s="65" t="s">
-        <v>658</v>
-      </c>
-      <c r="E166" s="63" t="s">
-        <v>657</v>
       </c>
       <c r="F166" s="63" t="s">
         <v>12</v>
@@ -23142,16 +23139,16 @@
         <v>845131</v>
       </c>
       <c r="B167" s="67" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C167" s="63" t="s">
+        <v>465</v>
+      </c>
+      <c r="D167" s="65" t="s">
         <v>466</v>
       </c>
-      <c r="D167" s="65" t="s">
+      <c r="E167" s="63" t="s">
         <v>467</v>
-      </c>
-      <c r="E167" s="63" t="s">
-        <v>468</v>
       </c>
       <c r="F167" s="63" t="s">
         <v>12</v>
@@ -23177,16 +23174,16 @@
         <v>845130</v>
       </c>
       <c r="B168" s="67" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C168" s="63" t="s">
+        <v>468</v>
+      </c>
+      <c r="D168" s="63" t="s">
         <v>469</v>
       </c>
-      <c r="D168" s="63" t="s">
+      <c r="E168" s="63" t="s">
         <v>470</v>
-      </c>
-      <c r="E168" s="63" t="s">
-        <v>471</v>
       </c>
       <c r="F168" s="63" t="s">
         <v>12</v>
@@ -23212,16 +23209,16 @@
         <v>845129</v>
       </c>
       <c r="B169" s="67" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C169" s="63" t="s">
+        <v>471</v>
+      </c>
+      <c r="D169" s="63" t="s">
         <v>472</v>
       </c>
-      <c r="D169" s="63" t="s">
+      <c r="E169" s="63" t="s">
         <v>473</v>
-      </c>
-      <c r="E169" s="63" t="s">
-        <v>474</v>
       </c>
       <c r="F169" s="63" t="s">
         <v>12</v>
@@ -23247,16 +23244,16 @@
         <v>845127</v>
       </c>
       <c r="B170" s="67" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C170" s="63" t="s">
+        <v>474</v>
+      </c>
+      <c r="D170" s="63" t="s">
         <v>475</v>
       </c>
-      <c r="D170" s="63" t="s">
+      <c r="E170" s="63" t="s">
         <v>476</v>
-      </c>
-      <c r="E170" s="63" t="s">
-        <v>477</v>
       </c>
       <c r="F170" s="63" t="s">
         <v>12</v>
@@ -23282,16 +23279,16 @@
         <v>845126</v>
       </c>
       <c r="B171" s="67" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C171" s="63" t="s">
+        <v>477</v>
+      </c>
+      <c r="D171" s="65" t="s">
         <v>478</v>
       </c>
-      <c r="D171" s="65" t="s">
+      <c r="E171" s="63" t="s">
         <v>479</v>
-      </c>
-      <c r="E171" s="63" t="s">
-        <v>480</v>
       </c>
       <c r="F171" s="63" t="s">
         <v>12</v>
@@ -23317,16 +23314,16 @@
         <v>845125</v>
       </c>
       <c r="B172" s="67" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C172" s="63" t="s">
+        <v>480</v>
+      </c>
+      <c r="D172" s="65" t="s">
         <v>481</v>
       </c>
-      <c r="D172" s="65" t="s">
+      <c r="E172" s="63" t="s">
         <v>482</v>
-      </c>
-      <c r="E172" s="63" t="s">
-        <v>483</v>
       </c>
       <c r="F172" s="63" t="s">
         <v>12</v>
@@ -23352,16 +23349,16 @@
         <v>845124</v>
       </c>
       <c r="B173" s="67" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C173" s="63" t="s">
+        <v>483</v>
+      </c>
+      <c r="D173" s="63" t="s">
         <v>484</v>
       </c>
-      <c r="D173" s="63" t="s">
+      <c r="E173" s="63" t="s">
         <v>485</v>
-      </c>
-      <c r="E173" s="63" t="s">
-        <v>486</v>
       </c>
       <c r="F173" s="63" t="s">
         <v>12</v>
@@ -23382,21 +23379,21 @@
         <v>43</v>
       </c>
     </row>
-    <row r="174" spans="1:11" s="65" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="67">
         <v>845123</v>
       </c>
       <c r="B174" s="67" t="s">
-        <v>446</v>
-      </c>
-      <c r="C174" s="91" t="s">
+        <v>445</v>
+      </c>
+      <c r="C174" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="D174" s="63" t="s">
         <v>487</v>
       </c>
-      <c r="D174" s="63" t="s">
+      <c r="E174" s="63" t="s">
         <v>488</v>
-      </c>
-      <c r="E174" s="63" t="s">
-        <v>489</v>
       </c>
       <c r="F174" s="63" t="s">
         <v>12</v>
@@ -24393,76 +24390,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="83"/>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
       <c r="L1" s="69"/>
     </row>
     <row r="3" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="14" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C4" s="15" t="s">
+        <v>632</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>633</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="17" t="s">
         <v>634</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>635</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>636</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="H4" s="18" t="s">
         <v>637</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C5" s="19" t="s">
+        <v>638</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>639</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>640</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="20" t="s">
+        <v>640</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>641</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>642</v>
       </c>
       <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C6" s="22" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="70" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -24485,258 +24482,258 @@
     </row>
     <row r="9" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="14" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C10" s="31" t="s">
+        <v>632</v>
+      </c>
+      <c r="D10" s="32" t="s">
         <v>633</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="E10" s="32" t="s">
         <v>634</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>635</v>
       </c>
       <c r="F10" s="32" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="32" t="s">
+        <v>644</v>
+      </c>
+      <c r="H10" s="32" t="s">
         <v>645</v>
       </c>
-      <c r="H10" s="32" t="s">
-        <v>646</v>
-      </c>
       <c r="I10" s="32" t="s">
+        <v>636</v>
+      </c>
+      <c r="J10" s="33" t="s">
         <v>637</v>
-      </c>
-      <c r="J10" s="33" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11" s="34" t="s">
+        <v>638</v>
+      </c>
+      <c r="D11" s="35" t="s">
         <v>639</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>640</v>
       </c>
       <c r="E11" s="35"/>
       <c r="F11" s="35" t="s">
+        <v>640</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>646</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>647</v>
+      </c>
+      <c r="I11" s="36" t="s">
         <v>641</v>
       </c>
-      <c r="G11" s="35" t="s">
-        <v>647</v>
-      </c>
-      <c r="H11" s="35" t="s">
+      <c r="J11" s="37"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C12" s="85" t="s">
+        <v>658</v>
+      </c>
+      <c r="D12" s="87" t="s">
         <v>648</v>
       </c>
-      <c r="I11" s="36" t="s">
-        <v>642</v>
-      </c>
-      <c r="J11" s="37"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C12" s="84" t="s">
-        <v>659</v>
-      </c>
-      <c r="D12" s="86" t="s">
-        <v>649</v>
-      </c>
       <c r="E12" s="38" t="s">
+        <v>660</v>
+      </c>
+      <c r="F12" s="39" t="s">
         <v>661</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="G12" s="39" t="s">
         <v>662</v>
-      </c>
-      <c r="G12" s="39" t="s">
-        <v>663</v>
       </c>
       <c r="H12" s="39"/>
       <c r="I12" s="20" t="s">
-        <v>643</v>
-      </c>
-      <c r="J12" s="88" t="s">
-        <v>660</v>
+        <v>642</v>
+      </c>
+      <c r="J12" s="89" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C13" s="85"/>
-      <c r="D13" s="87"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="88"/>
       <c r="E13" s="40"/>
       <c r="F13" s="39" t="s">
+        <v>663</v>
+      </c>
+      <c r="G13" s="39" t="s">
         <v>664</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="H13" s="39" t="s">
         <v>665</v>
       </c>
-      <c r="H13" s="39" t="s">
-        <v>666</v>
-      </c>
       <c r="I13" s="20" t="s">
-        <v>643</v>
-      </c>
-      <c r="J13" s="89"/>
+        <v>642</v>
+      </c>
+      <c r="J13" s="90"/>
       <c r="L13" s="41"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C14" s="85"/>
-      <c r="D14" s="87"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="88"/>
       <c r="E14" s="40"/>
       <c r="F14" s="39" t="s">
+        <v>666</v>
+      </c>
+      <c r="G14" s="39" t="s">
         <v>667</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>668</v>
       </c>
       <c r="H14" s="39"/>
       <c r="I14" s="20" t="s">
-        <v>643</v>
-      </c>
-      <c r="J14" s="89"/>
+        <v>642</v>
+      </c>
+      <c r="J14" s="90"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C15" s="85"/>
-      <c r="D15" s="87"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="88"/>
       <c r="E15" s="40"/>
       <c r="F15" s="39" t="s">
+        <v>668</v>
+      </c>
+      <c r="G15" s="39" t="s">
         <v>669</v>
-      </c>
-      <c r="G15" s="39" t="s">
-        <v>670</v>
       </c>
       <c r="H15" s="39"/>
       <c r="I15" s="20" t="s">
-        <v>643</v>
-      </c>
-      <c r="J15" s="89"/>
+        <v>642</v>
+      </c>
+      <c r="J15" s="90"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C16" s="85"/>
-      <c r="D16" s="87"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="88"/>
       <c r="E16" s="40"/>
       <c r="F16" s="39" t="s">
+        <v>670</v>
+      </c>
+      <c r="G16" s="39" t="s">
         <v>671</v>
-      </c>
-      <c r="G16" s="39" t="s">
-        <v>672</v>
       </c>
       <c r="H16" s="39"/>
       <c r="I16" s="20" t="s">
-        <v>643</v>
-      </c>
-      <c r="J16" s="89"/>
+        <v>642</v>
+      </c>
+      <c r="J16" s="90"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C17" s="85"/>
-      <c r="D17" s="87"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="88"/>
       <c r="E17" s="40"/>
       <c r="F17" s="39" t="s">
+        <v>672</v>
+      </c>
+      <c r="G17" s="39" t="s">
         <v>673</v>
-      </c>
-      <c r="G17" s="39" t="s">
-        <v>674</v>
       </c>
       <c r="H17" s="39"/>
       <c r="I17" s="20" t="s">
-        <v>643</v>
-      </c>
-      <c r="J17" s="89"/>
+        <v>642</v>
+      </c>
+      <c r="J17" s="90"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C18" s="71" t="s">
+        <v>653</v>
+      </c>
+      <c r="D18" s="72" t="s">
+        <v>652</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>648</v>
+      </c>
+      <c r="F18" s="39" t="s">
         <v>654</v>
-      </c>
-      <c r="D18" s="72" t="s">
-        <v>653</v>
-      </c>
-      <c r="E18" s="38" t="s">
-        <v>649</v>
-      </c>
-      <c r="F18" s="39" t="s">
-        <v>655</v>
       </c>
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
       <c r="I18" s="20" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J18" s="59" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="19" spans="3:10" ht="114.75" x14ac:dyDescent="0.2">
       <c r="C19" s="34" t="s">
+        <v>674</v>
+      </c>
+      <c r="D19" s="42" t="s">
         <v>675</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="E19" s="72" t="s">
+        <v>652</v>
+      </c>
+      <c r="F19" s="73" t="s">
         <v>676</v>
       </c>
-      <c r="E19" s="72" t="s">
-        <v>653</v>
-      </c>
-      <c r="F19" s="73" t="s">
+      <c r="G19" s="73" t="s">
         <v>677</v>
       </c>
-      <c r="G19" s="73" t="s">
+      <c r="H19" s="73" t="s">
         <v>678</v>
       </c>
-      <c r="H19" s="73" t="s">
+      <c r="I19" s="36" t="s">
         <v>679</v>
       </c>
-      <c r="I19" s="36" t="s">
+      <c r="J19" s="74" t="s">
         <v>680</v>
-      </c>
-      <c r="J19" s="74" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C20" s="34" t="s">
+        <v>681</v>
+      </c>
+      <c r="D20" s="42" t="s">
         <v>682</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="E20" s="42" t="s">
+        <v>675</v>
+      </c>
+      <c r="F20" s="36" t="s">
         <v>683</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>676</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>684</v>
       </c>
       <c r="G20" s="36"/>
       <c r="H20" s="36"/>
       <c r="I20" s="36" t="s">
+        <v>684</v>
+      </c>
+      <c r="J20" s="75" t="s">
         <v>685</v>
-      </c>
-      <c r="J20" s="75" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="21" spans="3:10" ht="51" x14ac:dyDescent="0.2">
       <c r="C21" s="34" t="s">
+        <v>686</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>675</v>
+      </c>
+      <c r="E21" s="72" t="s">
+        <v>675</v>
+      </c>
+      <c r="F21" s="73" t="s">
+        <v>688</v>
+      </c>
+      <c r="G21" s="36" t="s">
         <v>687</v>
       </c>
-      <c r="D21" s="44" t="s">
-        <v>676</v>
-      </c>
-      <c r="E21" s="72" t="s">
-        <v>676</v>
-      </c>
-      <c r="F21" s="73" t="s">
+      <c r="H21" s="36" t="s">
+        <v>665</v>
+      </c>
+      <c r="I21" s="36" t="s">
+        <v>684</v>
+      </c>
+      <c r="J21" s="75" t="s">
         <v>689</v>
-      </c>
-      <c r="G21" s="36" t="s">
-        <v>688</v>
-      </c>
-      <c r="H21" s="36" t="s">
-        <v>666</v>
-      </c>
-      <c r="I21" s="36" t="s">
-        <v>685</v>
-      </c>
-      <c r="J21" s="75" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.2">

</xml_diff>